<commit_message>
Blind model names and simplify human evaluation workflow
- Models now shown as "Model A, B, C, D" to prevent reviewer bias
- Blinding key saved to model_blinding_key.json (keep secret until done)
- Mapping: claude-opus-4.5=A, gemini-3-pro=B, gpt-5.1=C, kimi-k2=D
- Removed broken JS download button from HTML
- Added clear footer instructions: "use Excel to record scores"
- Workflow: HTML for reading translations, Excel for entering 1-5 scores

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/reports/eval_sheet_all_20251130.xlsx
+++ b/output/reports/eval_sheet_all_20251130.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -569,7 +569,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -629,7 +629,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -719,7 +719,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -809,7 +809,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1319,7 +1319,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1739,7 +1739,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2009,7 +2009,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2069,7 +2069,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2339,7 +2339,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2699,7 +2699,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2759,7 +2759,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2819,7 +2819,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2879,7 +2879,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3089,7 +3089,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -3239,7 +3239,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -3269,7 +3269,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3449,7 +3449,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3539,7 +3539,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3749,7 +3749,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3839,7 +3839,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3899,7 +3899,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3929,7 +3929,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3989,7 +3989,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -4139,7 +4139,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4259,7 +4259,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -4379,7 +4379,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -4439,7 +4439,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4469,7 +4469,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4499,7 +4499,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4529,7 +4529,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4559,7 +4559,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4589,7 +4589,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4619,7 +4619,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4739,7 +4739,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4799,7 +4799,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4829,7 +4829,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4859,7 +4859,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4889,7 +4889,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -5039,7 +5039,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -5069,7 +5069,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -5099,7 +5099,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -5129,7 +5129,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -5159,7 +5159,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -5219,7 +5219,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -5279,7 +5279,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -5369,7 +5369,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -5399,7 +5399,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -5459,7 +5459,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -5489,7 +5489,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -5519,7 +5519,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -5579,7 +5579,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -5639,7 +5639,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -5699,7 +5699,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -5729,7 +5729,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -5759,7 +5759,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -5819,7 +5819,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -5879,7 +5879,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -5909,7 +5909,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -5939,7 +5939,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -5969,7 +5969,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -6029,7 +6029,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -6119,7 +6119,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -6149,7 +6149,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -6209,7 +6209,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -6239,7 +6239,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -6269,7 +6269,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -6299,7 +6299,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -6329,7 +6329,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -6359,7 +6359,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -6389,7 +6389,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -6419,7 +6419,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -6479,7 +6479,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -6509,7 +6509,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -6539,7 +6539,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -6569,7 +6569,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -6599,7 +6599,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -6629,7 +6629,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
@@ -6659,7 +6659,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -6719,7 +6719,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -6749,7 +6749,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -6779,7 +6779,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -6809,7 +6809,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -6839,7 +6839,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D213" t="inlineStr">
@@ -6869,7 +6869,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -6899,7 +6899,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -6929,7 +6929,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
@@ -6959,7 +6959,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -6989,7 +6989,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
@@ -7019,7 +7019,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -7049,7 +7049,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -7079,7 +7079,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -7109,7 +7109,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -7139,7 +7139,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
@@ -7169,7 +7169,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -7199,7 +7199,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -7229,7 +7229,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -7259,7 +7259,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -7289,7 +7289,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -7319,7 +7319,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -7349,7 +7349,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -7379,7 +7379,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -7409,7 +7409,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -7439,7 +7439,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -7469,7 +7469,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -7499,7 +7499,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -7529,7 +7529,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -7559,7 +7559,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -7589,7 +7589,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -7619,7 +7619,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -7649,7 +7649,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -7679,7 +7679,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -7709,7 +7709,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -7739,7 +7739,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -7769,7 +7769,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -7799,7 +7799,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -7829,7 +7829,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -7859,7 +7859,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -7889,7 +7889,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -7919,7 +7919,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -7949,7 +7949,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -7979,7 +7979,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -8009,7 +8009,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
@@ -8039,7 +8039,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -8069,7 +8069,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -8099,7 +8099,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -8129,7 +8129,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -8159,7 +8159,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -8189,7 +8189,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -8219,7 +8219,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -8249,7 +8249,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -8279,7 +8279,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
@@ -8309,7 +8309,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -8339,7 +8339,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -8369,7 +8369,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
@@ -8399,7 +8399,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
@@ -8429,7 +8429,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -8459,7 +8459,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
@@ -8489,7 +8489,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -8519,7 +8519,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
@@ -8549,7 +8549,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -8579,7 +8579,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -8609,7 +8609,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -8639,7 +8639,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -8669,7 +8669,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -8699,7 +8699,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -8729,7 +8729,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
@@ -8759,7 +8759,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -8789,7 +8789,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -8819,7 +8819,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D279" t="inlineStr">
@@ -8849,7 +8849,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D280" t="inlineStr">
@@ -8879,7 +8879,7 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D281" t="inlineStr">
@@ -8909,7 +8909,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D282" t="inlineStr">
@@ -8939,7 +8939,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D283" t="inlineStr">
@@ -8969,7 +8969,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -8999,7 +8999,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
@@ -9029,7 +9029,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D286" t="inlineStr">
@@ -9059,7 +9059,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>gpt-5.1</t>
+          <t>Model C</t>
         </is>
       </c>
       <c r="D287" t="inlineStr">
@@ -9089,7 +9089,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>claude-opus-4.5</t>
+          <t>Model A</t>
         </is>
       </c>
       <c r="D288" t="inlineStr">
@@ -9119,7 +9119,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>gemini-3-pro</t>
+          <t>Model B</t>
         </is>
       </c>
       <c r="D289" t="inlineStr">
@@ -9149,7 +9149,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D290" t="inlineStr">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -9239,7 +9239,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D293" t="inlineStr">
@@ -9269,7 +9269,7 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D294" t="inlineStr">
@@ -9299,7 +9299,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D295" t="inlineStr">
@@ -9329,7 +9329,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D296" t="inlineStr">
@@ -9359,7 +9359,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D297" t="inlineStr">
@@ -9389,7 +9389,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D298" t="inlineStr">
@@ -9419,7 +9419,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D299" t="inlineStr">
@@ -9449,7 +9449,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D300" t="inlineStr">
@@ -9479,7 +9479,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D301" t="inlineStr">
@@ -9509,7 +9509,7 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D302" t="inlineStr">
@@ -9539,7 +9539,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D303" t="inlineStr">
@@ -9569,7 +9569,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D304" t="inlineStr">
@@ -9599,7 +9599,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D305" t="inlineStr">
@@ -9629,7 +9629,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D306" t="inlineStr">
@@ -9659,7 +9659,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
@@ -9689,7 +9689,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D308" t="inlineStr">
@@ -9719,7 +9719,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D309" t="inlineStr">
@@ -9749,7 +9749,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D310" t="inlineStr">
@@ -9779,7 +9779,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D311" t="inlineStr">
@@ -9809,7 +9809,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D312" t="inlineStr">
@@ -9839,7 +9839,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
@@ -9869,7 +9869,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D314" t="inlineStr">
@@ -9899,7 +9899,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D315" t="inlineStr">
@@ -9929,7 +9929,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
@@ -9959,7 +9959,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
@@ -9989,7 +9989,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
@@ -10019,7 +10019,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
@@ -10049,7 +10049,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
@@ -10079,7 +10079,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D321" t="inlineStr">
@@ -10109,7 +10109,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
@@ -10139,7 +10139,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D323" t="inlineStr">
@@ -10169,7 +10169,7 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D324" t="inlineStr">
@@ -10199,7 +10199,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
@@ -10229,7 +10229,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
@@ -10259,7 +10259,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
@@ -10289,7 +10289,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
@@ -10319,7 +10319,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D329" t="inlineStr">
@@ -10349,7 +10349,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
@@ -10379,7 +10379,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
@@ -10409,7 +10409,7 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D332" t="inlineStr">
@@ -10439,7 +10439,7 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D333" t="inlineStr">
@@ -10469,7 +10469,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D334" t="inlineStr">
@@ -10499,7 +10499,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D335" t="inlineStr">
@@ -10529,7 +10529,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">
@@ -10559,7 +10559,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
@@ -10589,7 +10589,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D338" t="inlineStr">
@@ -10619,7 +10619,7 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D339" t="inlineStr">
@@ -10649,7 +10649,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
@@ -10679,7 +10679,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
@@ -10709,7 +10709,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
@@ -10739,7 +10739,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
@@ -10769,7 +10769,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
@@ -10799,7 +10799,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
@@ -10829,7 +10829,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
@@ -10859,7 +10859,7 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
@@ -10889,7 +10889,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
@@ -10919,7 +10919,7 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
@@ -10949,7 +10949,7 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
@@ -10979,7 +10979,7 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D351" t="inlineStr">
@@ -11009,7 +11009,7 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D352" t="inlineStr">
@@ -11039,7 +11039,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
@@ -11069,7 +11069,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
@@ -11099,7 +11099,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
@@ -11129,7 +11129,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D356" t="inlineStr">
@@ -11159,7 +11159,7 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D357" t="inlineStr">
@@ -11189,7 +11189,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D358" t="inlineStr">
@@ -11219,7 +11219,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D359" t="inlineStr">
@@ -11249,7 +11249,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D360" t="inlineStr">
@@ -11279,7 +11279,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D361" t="inlineStr">
@@ -11309,7 +11309,7 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D362" t="inlineStr">
@@ -11339,7 +11339,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D363" t="inlineStr">
@@ -11369,7 +11369,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D364" t="inlineStr">
@@ -11399,7 +11399,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">
@@ -11429,7 +11429,7 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
@@ -11459,7 +11459,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D367" t="inlineStr">
@@ -11489,7 +11489,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D368" t="inlineStr">
@@ -11519,7 +11519,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D369" t="inlineStr">
@@ -11549,7 +11549,7 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D370" t="inlineStr">
@@ -11579,7 +11579,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D371" t="inlineStr">
@@ -11609,7 +11609,7 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D372" t="inlineStr">
@@ -11639,7 +11639,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D373" t="inlineStr">
@@ -11669,7 +11669,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D374" t="inlineStr">
@@ -11699,7 +11699,7 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D375" t="inlineStr">
@@ -11729,7 +11729,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D376" t="inlineStr">
@@ -11759,7 +11759,7 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D377" t="inlineStr">
@@ -11789,7 +11789,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D378" t="inlineStr">
@@ -11819,7 +11819,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D379" t="inlineStr">
@@ -11849,7 +11849,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D380" t="inlineStr">
@@ -11879,7 +11879,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D381" t="inlineStr">
@@ -11909,7 +11909,7 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D382" t="inlineStr">
@@ -11939,7 +11939,7 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D383" t="inlineStr">
@@ -11969,7 +11969,7 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D384" t="inlineStr">
@@ -11999,7 +11999,7 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>kimi-k2</t>
+          <t>Model D</t>
         </is>
       </c>
       <c r="D385" t="inlineStr">

</xml_diff>